<commit_message>
extraction données et labels DF dans un dictionnaire (et retrait d'une ligne parasite dans le fichier excel 2023 et 2024)
</commit_message>
<xml_diff>
--- a/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
+++ b/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F896C3-9030-463A-931A-77C4F77AB9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-DF-Tri" sheetId="5" r:id="rId1"/>
@@ -18,10 +19,21 @@
     <sheet name="2023-DRI-Tri" sheetId="4" r:id="rId9"/>
     <sheet name="2023-DRI-Annuel" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -408,7 +420,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,14 +653,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -935,7 +947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -945,14 +957,14 @@
       <selection activeCell="A9" sqref="A9:K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -978,7 +990,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>55</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>59</v>
       </c>
@@ -1056,7 +1068,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>61</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>63</v>
       </c>
@@ -1119,16 +1131,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1157,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -1168,16 +1180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1212,7 +1224,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>52</v>
       </c>
@@ -1254,21 +1266,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="10" width="17.7109375" customWidth="1"/>
+    <col min="5" max="10" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1351,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1371,11 +1383,11 @@
         <v>25</v>
       </c>
       <c r="K3" s="19">
-        <f t="shared" ref="K3:K4" si="0">SUM(E3:J3)</f>
+        <f t="shared" ref="K3" si="0">SUM(E3:J3)</f>
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1415,21 +1427,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="10" width="17.7109375" customWidth="1"/>
+    <col min="5" max="10" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1643,7 +1655,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1753,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1870,21 +1882,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="10" width="17.7109375" customWidth="1"/>
+    <col min="5" max="10" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1988,7 +2000,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -2098,7 +2110,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2318,7 +2330,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>745000</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2490,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2498,16 +2510,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2539,7 +2551,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -2577,22 +2589,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:AF10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="16" width="12.7109375" customWidth="1"/>
-    <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="16" width="12.7265625" customWidth="1"/>
+    <col min="29" max="29" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2642,30 +2654,63 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="14">
+        <f>SUM(F2:P2)</f>
+        <v>132</v>
+      </c>
+      <c r="F2" s="14">
+        <v>10</v>
+      </c>
+      <c r="G2" s="14">
+        <v>3</v>
+      </c>
+      <c r="H2" s="14">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14">
+        <v>5</v>
+      </c>
+      <c r="J2" s="14">
+        <v>4</v>
+      </c>
+      <c r="K2" s="5">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5">
+        <v>15</v>
+      </c>
+      <c r="M2" s="5">
+        <v>20</v>
+      </c>
+      <c r="N2" s="5">
+        <v>20</v>
+      </c>
+      <c r="O2" s="5">
+        <v>15</v>
+      </c>
+      <c r="P2" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -2673,109 +2718,108 @@
       <c r="D3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="14">
-        <f>SUM(F3:P3)</f>
-        <v>132</v>
+      <c r="E3" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G3" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3" s="14">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I3" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J3" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K3" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L3" s="5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M3" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="O3" s="5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P3" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="14">
+        <v>80</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="P4" s="5">
         <v>2</v>
       </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="E5" s="14">
+        <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>54</v>
@@ -2792,31 +2836,31 @@
       <c r="J5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5">
-        <v>1</v>
-      </c>
-      <c r="N5" s="5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="5">
-        <v>2</v>
-      </c>
-      <c r="P5" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -2825,7 +2869,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="14">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>54</v>
@@ -2858,56 +2902,6 @@
         <v>54</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="14">
-        <v>30</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P7" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2918,16 +2912,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3022,7 +3016,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
@@ -3130,21 +3124,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3170,7 +3164,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
@@ -3196,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -3222,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -3248,7 +3242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
@@ -3274,7 +3268,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -3300,7 +3294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
extraction données et labels dans un dictionnaire, extraction des equivalences entre anciens et nouveaux indicateurs
</commit_message>
<xml_diff>
--- a/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
+++ b/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F896C3-9030-463A-931A-77C4F77AB9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF1A8A-568A-4ABB-823D-614F5CB20EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-DF-Tri" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="125">
   <si>
     <t>Indicateur</t>
   </si>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
@@ -1886,7 +1886,7 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2592,9 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2915,13 +2913,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3127,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajout fichier data_historique pour extraire les données historique
</commit_message>
<xml_diff>
--- a/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
+++ b/assets/Saisie-2023-INDICATEUR-DE-SUIVI-Ti-2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF1A8A-568A-4ABB-823D-614F5CB20EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6E06EF-FEBF-4203-B194-4F7A99163CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-DF-Tri" sheetId="5" r:id="rId1"/>
@@ -954,7 +954,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1270,7 +1270,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1886,7 +1886,7 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2592,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2913,7 +2913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>